<commit_message>
changing table id=>class to allow custom table ids to keep track of the table origin of each model instance
</commit_message>
<xml_diff>
--- a/examples/address_book/schema_and_data.xlsx
+++ b/examples/address_book/schema_and_data.xlsx
@@ -293,10 +293,10 @@
     <t>'!!People'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-14 13:19:04'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-03-14 13:19:04' objTablesVersion='0.0.8'</t>
+    <t>!!!ObjTables objTablesVersion='0.0.9' date='2020-04-27 01:05:01'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -320,7 +320,7 @@
     <t>People</t>
   </si>
   <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-14 13:19:04' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -428,7 +428,7 @@
     <t>zip_code</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='column' id='Company' name='Companies' date='2020-03-14 13:19:04' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' tableFormat='column' class='Company' name='Companies' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
   </si>
   <si>
     <t>Apple</t>
@@ -518,7 +518,7 @@
     <t>US</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' id='Person' name='People' date='2020-03-14 13:19:04' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Person' name='People' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
   </si>
   <si>
     <t>!Company</t>

</xml_diff>

<commit_message>
renaming EmpiricalFormulaAttribute->ChemicalFormulaAttribute; enabling searializing *-to-many relationships to CSV and TSV tables; adding ReactionEquationAttribute and ListAttribute; adding metabolomics example
</commit_message>
<xml_diff>
--- a/examples/address_book/schema_and_data.xlsx
+++ b/examples/address_book/schema_and_data.xlsx
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
   <si>
     <t>'!!_Schema'!A1</t>
   </si>
@@ -293,10 +293,10 @@
     <t>'!!People'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='0.0.9' date='2020-04-27 01:05:01'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
+    <t>!!!ObjTables objTablesVersion='1.0.0' date='2020-03-14 13:19:04'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -320,7 +320,7 @@
     <t>People</t>
   </si>
   <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -359,18 +359,27 @@
     <t>OneToOne('Address', related_name='company')</t>
   </si>
   <si>
+    <t>Address</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
     <t>String(primary=True, unique=True)</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>url</t>
   </si>
   <si>
     <t>Url</t>
   </si>
   <si>
+    <t>URL</t>
+  </si>
+  <si>
     <t>Person</t>
   </si>
   <si>
@@ -392,19 +401,25 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Email address</t>
+  </si>
+  <si>
     <t>phone_number</t>
   </si>
   <si>
     <t>String</t>
   </si>
   <si>
+    <t>Phone number</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
     <t>Enum([('family', 1), ('friend', 2), ('business', 3)])</t>
   </si>
   <si>
-    <t>Address</t>
+    <t>Type</t>
   </si>
   <si>
     <t>multiple_cells</t>
@@ -416,19 +431,34 @@
     <t>city</t>
   </si>
   <si>
+    <t>City</t>
+  </si>
+  <si>
     <t>country</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
     <t>state</t>
   </si>
   <si>
+    <t>State</t>
+  </si>
+  <si>
     <t>street</t>
   </si>
   <si>
+    <t>Street</t>
+  </si>
+  <si>
     <t>zip_code</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='column' class='Company' name='Companies' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
+    <t>Zip code</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='column' class='Company' name='Companies' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>Apple</t>
@@ -518,7 +548,7 @@
     <t>US</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Person' name='People' date='2020-04-27 01:05:01' objTablesVersion='0.0.9'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Person' name='People' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Company</t>
@@ -1118,13 +1148,15 @@
       <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="15.01" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>23</v>
@@ -1133,15 +1165,17 @@
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="15.01" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>23</v>
@@ -1150,25 +1184,27 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="15.01" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
@@ -1183,201 +1219,223 @@
         <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="15.01" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="15.01" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="15.01" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="15.01" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15.01" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="15.01" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="15.01" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="15.01" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.01" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.01" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.01" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
@@ -1411,7 +1469,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1425,134 +1483,134 @@
         <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.01" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.01" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1663,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1624,19 +1682,19 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.01" customHeight="1">
@@ -1647,156 +1705,156 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.01" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.01" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.01" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.01" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugging examples XLSX files for Microsoft Excel
</commit_message>
<xml_diff>
--- a/examples/address_book/schema_and_data.xlsx
+++ b/examples/address_book/schema_and_data.xlsx
@@ -21,266 +21,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.
-Value must be unique.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 65535 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.
-Value must be unique.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.
-Value must be unique.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Select one of "family", "friend", "business".</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Select a value from "!!Company:2" or blank.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.
-Value must be unique.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a string.
-Value must be less than or equal to 255 characters.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
   <si>
@@ -293,10 +33,10 @@
     <t>'!!People'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='1.0.0' date='2020-03-14 13:19:04'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
+    <t>!!!ObjTables objTablesVersion='1.0.1' date='2020-03-14 13:19:04'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-03-14 13:19:04' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -320,7 +60,7 @@
     <t>People</t>
   </si>
   <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-14 13:19:04' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -458,7 +198,7 @@
     <t>Zip code</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='column' class='Company' name='Companies' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Data' tableFormat='column' class='Company' name='Companies' date='2020-03-14 13:19:04' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>Apple</t>
@@ -548,7 +288,7 @@
     <t>US</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Person' name='People' date='2020-03-14 13:19:04' objTablesVersion='1.0.0'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Person' name='People' date='2020-03-14 13:19:04' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Company</t>
@@ -606,19 +346,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -677,23 +411,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1004,54 +737,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1083,361 +816,361 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
@@ -1468,148 +1201,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.01" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1642,7 +1375,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1662,198 +1394,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.01" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.01" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.01" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.01" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.01" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1896,6 +1628,5 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>